<commit_message>
Preserve cell formatting (percentages, currency, dates) in output file
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -16,7 +16,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="165" formatCode="$#,##0"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +59,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,193 +445,193 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Employee_ID</t>
+          <t>Employee</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Name</t>
+          <t>Department</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Department</t>
+          <t>Salary</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Salary</t>
+          <t>Bonus</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Years_Experience</t>
+          <t>Performance</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Quota Met</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Email</t>
+          <t>Start Date</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Hours Worked</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1001</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Alice Johnson</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>John Smith</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
           <t>Engineering</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>75000</v>
-      </c>
-      <c r="E2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>john@example.com</t>
-        </is>
+      <c r="C2" s="3" t="n">
+        <v>85000</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>8500</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>44270</v>
+      </c>
+      <c r="H2" s="6" t="n">
+        <v>42.5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>1002</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Bob Smith</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Jane Doe</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>65000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>San Francisco</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>jane@example.com</t>
-        </is>
+      <c r="C3" s="3" t="n">
+        <v>72000</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>10800</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>43668</v>
+      </c>
+      <c r="H3" s="6" t="n">
+        <v>38.75</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>1003</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Carol White</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bob Johnson</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Engineering</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>80000</v>
-      </c>
-      <c r="E4" t="n">
-        <v>7</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Boston</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>bob@example.com</t>
-        </is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>68000</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>5100</v>
+      </c>
+      <c r="E4" s="4" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>44571</v>
+      </c>
+      <c r="H4" s="6" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>1004</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>David Brown</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alice Williams</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>HR</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>55000</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>New York</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>alice@example.com</t>
-        </is>
+          <t>Engineering</t>
+        </is>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>92000</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>11040</v>
+      </c>
+      <c r="E5" s="4" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>43409</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <v>45.25</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>1005</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Eva Martinez</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Charlie Brown</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
           <t>Sales</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>70000</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Chicago</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>charlie@example.com</t>
-        </is>
+      <c r="C6" s="3" t="n">
+        <v>78000</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>9360</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>44000</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <v>39.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>